<commit_message>
add User info page
</commit_message>
<xml_diff>
--- a/lang values.xlsx
+++ b/lang values.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>key</t>
   </si>
@@ -52,6 +52,45 @@
   </si>
   <si>
     <t>Регистрация</t>
+  </si>
+  <si>
+    <t>system.common.streetName</t>
+  </si>
+  <si>
+    <t>Street name</t>
+  </si>
+  <si>
+    <t>Улица/блок</t>
+  </si>
+  <si>
+    <t>Улица</t>
+  </si>
+  <si>
+    <t>system.common.Neighborhood</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>Квартал</t>
+  </si>
+  <si>
+    <t>Микрорайон</t>
+  </si>
+  <si>
+    <t>system.common.City</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Град</t>
+  </si>
+  <si>
+    <t>Город</t>
+  </si>
+  <si>
+    <t>system.common.unrequired</t>
   </si>
 </sst>
 </file>
@@ -372,16 +411,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F4"/>
+  <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -427,6 +466,53 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add,edit user details done
</commit_message>
<xml_diff>
--- a/lang values.xlsx
+++ b/lang values.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>key</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>system.common.unrequired</t>
+  </si>
+  <si>
+    <t>system.common.edit</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F8"/>
+  <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +516,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>